<commit_message>
2021-03-17_Case List에서 일치 Case 찾기
</commit_message>
<xml_diff>
--- a/searchTable.xlsx
+++ b/searchTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KYEONGRYUN_KIM\gitRepos\Python-WebCrawling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9731350-F20A-4B35-9107-823B4AF35B56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85854DCA-AE75-4525-A7AC-A651BEBBCBA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24154" yWindow="-113" windowWidth="24267" windowHeight="13148" xr2:uid="{3FE82648-1DF1-46B9-8797-19653107D79B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Client</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -55,11 +55,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ELM3DS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Ericsson</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Elm 3DS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Patent</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -424,27 +432,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C75F2755-FC7F-4801-9B6A-A38559A71AF8}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.2" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="18.69921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -452,20 +463,26 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Jump2Case function 구현 & 에러 발생
</commit_message>
<xml_diff>
--- a/searchTable.xlsx
+++ b/searchTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KYEONGRYUN_KIM\gitRepos\Python-WebCrawling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB839A98-F77D-49B8-9C74-BC61D7D55F17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90127B50-9239-4765-A1BE-7CE02F3204E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-48196" yWindow="2529" windowWidth="24267" windowHeight="13148" xr2:uid="{3FE82648-1DF1-46B9-8797-19653107D79B}"/>
+    <workbookView xWindow="-24154" yWindow="-113" windowWidth="24267" windowHeight="13148" xr2:uid="{3FE82648-1DF1-46B9-8797-19653107D79B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -443,13 +443,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.2" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="18.69921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">

</xml_diff>